<commit_message>
OVT-9159 yksikkötesti lisää tuonnille
</commit_message>
<xml_diff>
--- a/src/test/resources/kustom_erillishaku.xlsx
+++ b/src/test/resources/kustom_erillishaku.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11720" yWindow="2320" windowWidth="25600" windowHeight="18020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,31 +19,60 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>sukunimi</t>
-  </si>
-  <si>
-    <t>etunimi</t>
-  </si>
-  <si>
-    <t>hetu</t>
-  </si>
-  <si>
-    <t>11.11.2011</t>
-  </si>
-  <si>
-    <t>HYLATTY</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+  <si>
+    <t>Hakkarainen</t>
+  </si>
+  <si>
+    <t>Tuomas</t>
+  </si>
+  <si>
+    <t>010101-123N</t>
+  </si>
+  <si>
+    <t>1.1.1901</t>
+  </si>
+  <si>
+    <t>HYVAKSYTTY</t>
+  </si>
+  <si>
+    <t>KESKEN</t>
+  </si>
+  <si>
+    <t>JULKAISTAVISSA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -66,13 +95,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -402,33 +436,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>